<commit_message>
RE-Framework RPA09 카카오맵유류비검증 - Performer 구현
</commit_message>
<xml_diff>
--- a/RE-Framework_RPA09_카카오맵유류비검증_박채연/RPA09_카카오맵유류비검증_Performer/Data/Config.xlsx
+++ b/RE-Framework_RPA09_카카오맵유류비검증_박채연/RPA09_카카오맵유류비검증_Performer/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sein\Documents\REFramework\RE-Framework_RPA09_카카오맵유류비검증_박채연\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sein\Documents\REFramework\RE-Framework_RPA09_카카오맵유류비검증_박채연\RPA09_카카오맵유류비검증_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95714EA-F055-43B5-98E7-C01E3D8B3FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897D912A-77F3-4FDF-9711-D67DFFAD086C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
   </bookViews>
@@ -22,12 +22,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -337,9 +348,6 @@
   <si>
     <t>OrchestratorQueueName</t>
     <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -644,6 +652,54 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
+    <t>Url</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>유류비검증_result_temp.xlsx</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>InputFolderId</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>OutputFolderId</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>유류비검증_Dispatcher_temp.xlsx</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Data\Input\</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Data\Output\</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Data\ExPath\</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0} {1} 처리 결과 : {2}</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://map.kakao.com/</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -678,50 +734,22 @@
       </rPr>
       <t>❤️❤️</t>
     </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Url</t>
     <phoneticPr fontId="13"/>
   </si>
   <si>
-    <t>유류비검증_result_temp.xlsx</t>
+    <t>EmployeeList_Queue</t>
     <phoneticPr fontId="13"/>
   </si>
   <si>
-    <t>InputFolderId</t>
+    <t>mangoperry2015@gmail.com's workspace</t>
     <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>OutputFolderId</t>
-    <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>유류비검증_Dispatcher_temp.xlsx</t>
-    <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>Data\Input\</t>
-    <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>Data\Output\</t>
-    <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>Data\ExPath\</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0} {1} 처리 결과 : {2}</t>
-    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,6 +872,14 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -959,9 +995,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1014,6 +1047,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1364,7 +1400,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -1390,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1398,20 +1434,20 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>101</v>
+      <c r="B3" s="26" t="s">
+        <v>100</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="31.2">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1436,10 +1472,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
@@ -1456,10 +1492,12 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1472,10 +1510,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
@@ -1483,10 +1521,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1494,8 +1532,8 @@
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>110</v>
+      <c r="B13" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>16</v>
@@ -1522,7 +1560,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1531,25 +1569,25 @@
         <v>20</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="11"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="46.8">
       <c r="A18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="409.6">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>74</v>
+      <c r="B19" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>22</v>
@@ -1559,11 +1597,11 @@
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1578,7 +1616,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1587,26 +1625,26 @@
         <v>27</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="29" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="30"/>
@@ -1616,85 +1654,85 @@
         <v>70</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="46.8">
       <c r="A27" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1717,7 +1755,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -1728,338 +1766,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" ht="26.4">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="26.4">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="23">
+        <v>5</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="24">
-        <v>5</v>
-      </c>
-      <c r="C4" s="22" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="17">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="17">
+        <v>30000</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="17">
+        <v>120000</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="17">
+        <v>15000</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="17">
+        <v>60000</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="16" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="18">
-        <v>5000</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="18">
-        <v>30000</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="18">
-        <v>120000</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="18">
-        <v>1000</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="18">
-        <v>15000</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="18">
-        <v>60000</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="18">
-        <v>0.8</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="17" t="s">
+      <c r="B24" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="C24" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="17" t="s">
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="16" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="17" t="s">
+      <c r="B25" s="17">
+        <v>2</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="18">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="17">
         <v>2</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="18">
-        <v>2</v>
-      </c>
-      <c r="C26" s="17" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="26.4">
+      <c r="A27" s="16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="26.4">
-      <c r="A27" s="17" t="s">
+      <c r="B27" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="17"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="17"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="17"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="14"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -2069,10 +2107,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C45133-1F58-4797-8585-3B6A73A476FF}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -2084,21 +2122,203 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
RE-Framework RPA09 카카오맵유류비검증 - Performer 예외처리
</commit_message>
<xml_diff>
--- a/RE-Framework_RPA09_카카오맵유류비검증_박채연/RPA09_카카오맵유류비검증_Performer/Data/Config.xlsx
+++ b/RE-Framework_RPA09_카카오맵유류비검증_박채연/RPA09_카카오맵유류비검증_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sein\Documents\REFramework\RE-Framework_RPA09_카카오맵유류비검증_박채연\RPA09_카카오맵유류비검증_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897D912A-77F3-4FDF-9711-D67DFFAD086C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7B13E6-978D-41BD-832A-3460CC379165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80601F42-B835-411D-B6F1-01869415BCDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -358,184 +358,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;RPA_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp;nbsp;결과 안내 메일입니다.&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;결과 데이터를&amp;nbsp;확인하여 주시기 바랍니다.&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;감사합니다.&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{2}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;/span&gt;&lt;/p&gt;
-&lt;table cellspacing="0" cellpadding="0" border="1" style="width: 776px; height: 60px; font-size: 10pt; border-width: 0px; border-color: rgb(0, 0, 0); border-collapse: collapse; border-style: solid; background-color: rgb(255, 255, 255); background-image: none; background-repeat: repeat; background-position: 0% 0%;" class=""&gt;
-&lt;tbody&gt;
-&lt;tr&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;총건수&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;처리건수&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" colspan="1" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;미처리건수&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;th style="width: 154px; height: 29px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" colspan="1" scope="col"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;비&amp;nbsp; &amp;nbsp;고&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
-&lt;/tr&gt;
-&lt;tr&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{3}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt; color: rgb(0, 0, 255); font-weight: bold;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{4}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;" colspan="1"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0); font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{5}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;td style="width: 154px; height: 30px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;" colspan="1"&gt;
-&lt;p style="text-align: center;"&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;&amp;nbsp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{6}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
-&lt;/tr&gt;</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>{0}=날짜
 {1}=과제명 dicConfig("과제명").ToString
 {2}=기준정보시트 &amp; 다운로드대상시트 &amp; 20.다운로드대상폴더
@@ -632,26 +454,6 @@
     <phoneticPr fontId="13"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-      </rPr>
-      <t>RPA09_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>카카오맵유류비검증</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>Url</t>
     <phoneticPr fontId="13"/>
   </si>
@@ -700,13 +502,22 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="3"/>
-      </rPr>
-      <t>❤️❤️</t>
+    <t>EmployeeList_Queue</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>mangoperry2015@gmail.com's workspace</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>♥♥</t>
     </r>
     <r>
       <rPr>
@@ -714,7 +525,7 @@
         <rFont val="Calibri"/>
         <family val="3"/>
       </rPr>
-      <t>RPA09_</t>
+      <t xml:space="preserve">RPA09 </t>
     </r>
     <r>
       <rPr>
@@ -724,32 +535,190 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>카카오맵유류비검증</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="3"/>
-      </rPr>
-      <t>❤️❤️</t>
+      <t>카카오맵 유류비 검증</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>♥♥</t>
     </r>
     <phoneticPr fontId="13"/>
   </si>
   <si>
-    <t>EmployeeList_Queue</t>
-    <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>mangoperry2015@gmail.com's workspace</t>
-    <phoneticPr fontId="13"/>
+    <t>RPA_02_기업은행유류비검증결과</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;p&gt;
+&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{0} {1} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>결과 안내 메일입니다.&lt;/span&gt;
+&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;결과 데이터를 확인하여 주시기 바랍니다.&lt;/span&gt;
+&lt;/p&gt;
+&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;감사합니다.&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{2}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;
+&lt;table cellspacing="0" cellpadding="0" border="1" style="width: 776px; height: 60px; font-size: 10pt; border-width: 0px; border-color: rgb(0, 0, 0); border-collapse: collapse; border-style: solid; background-color: rgb(255, 255, 255);" class=""&gt;
+&lt;tbody&gt;
+&lt;tr&gt;
+&lt;th style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" scope="col"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;총건수&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
+&lt;th style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" scope="col"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;처리건수&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
+&lt;th style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" colspan="1" scope="col"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;미처리건수&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
+&lt;th style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid; background-color: rgb(207, 226, 243);" colspan="1" scope="col"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;비고&lt;/span&gt;&lt;/p&gt;&lt;/th&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{3}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
+&lt;td style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt; color: rgb(0, 0, 255); font-weight: bold;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{4}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
+&lt;td style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;" colspan="1"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0); font-weight: bold; font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{5}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
+&lt;td style="width: 154px; height: 28px; border-width: 1px; border-color: rgb(0, 0, 0); border-style: solid;" colspan="1"&gt;
+&lt;p style="text-align: center;"&gt;&lt;span style="font-family: &amp;quot;Malgun Gothic&amp;quot;; font-size: 12pt;"&gt;&amp;nbsp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{6}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;&lt;/td&gt;
+&lt;/tr&gt;
+&lt;/tbody&gt;
+&lt;/table&gt;</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,11 +827,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Segoe UI Emoji"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Calibri"/>
       <family val="3"/>
     </font>
@@ -1045,10 +1009,10 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1400,7 +1364,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -1426,7 +1390,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1435,19 +1399,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="31.2">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1472,10 +1436,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
@@ -1492,10 +1456,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>12</v>
@@ -1510,10 +1474,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
@@ -1521,10 +1485,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1533,7 +1497,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>16</v>
@@ -1560,7 +1524,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1573,21 +1537,21 @@
     </row>
     <row r="18" spans="1:3" ht="46.8">
       <c r="A18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="409.6">
+    </row>
+    <row r="19" spans="1:3" ht="188.4" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>22</v>
@@ -1601,7 +1565,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1616,7 +1580,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1625,10 +1589,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1654,7 +1618,7 @@
         <v>70</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>71</v>
@@ -1662,11 +1626,11 @@
     </row>
     <row r="27" spans="1:3" ht="46.8">
       <c r="A27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1794,13 +1758,13 @@
     </row>
     <row r="4" spans="1:3" ht="26.4">
       <c r="A4" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="23">
         <v>5</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1990,46 +1954,46 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="C24" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" s="17">
         <v>2</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="17">
         <v>2</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="26.4">
       <c r="A27" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="17" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2075,7 +2039,7 @@
     <row r="36" spans="1:3">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" s="13"/>
     </row>
@@ -2126,10 +2090,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>68</v>
@@ -2137,13 +2101,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="C2" s="27" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -2155,7 +2119,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>

</xml_diff>